<commit_message>
Made the conclusion and spelled "Shakespeare" right.
</commit_message>
<xml_diff>
--- a/CSC430 Proj.xlsx
+++ b/CSC430 Proj.xlsx
@@ -1,49 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/logancamp/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonyj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F9672A-A651-2449-B84E-1FF31CE8DEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352F258F-7AB4-47B4-B247-D7A1C2EFCF7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{194B7978-61BF-E746-BFF1-312F519DEFB4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{194B7978-61BF-E746-BFF1-312F519DEFB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -87,20 +76,20 @@
     <t>Text</t>
   </si>
   <si>
-    <t>Shakespear</t>
-  </si>
-  <si>
     <t>Lottery</t>
   </si>
   <si>
     <t>Titanic</t>
+  </si>
+  <si>
+    <t>Shakespeare</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -255,16 +244,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -281,6 +264,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,7 +326,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> TIme Shakespear</a:t>
+              <a:t> TIme Shakespeare</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1874,7 +1863,7 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Shakespear</c:v>
+                  <c:v>Shakespeare</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Titanic</c:v>
@@ -1939,7 +1928,7 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Shakespear</c:v>
+                  <c:v>Shakespeare</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Titanic</c:v>
@@ -2004,7 +1993,7 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Shakespear</c:v>
+                  <c:v>Shakespeare</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Titanic</c:v>
@@ -4875,44 +4864,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3516C63E-AE4E-114B-B95F-EE1600AC9405}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="99" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="14" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2">
@@ -4930,14 +4919,14 @@
       <c r="H2">
         <v>0.30901499999999998</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="13">
         <f>AVERAGE(D2:H2)</f>
         <v>0.30481060000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
+    <row r="3" spans="1:9">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D3">
@@ -4955,45 +4944,45 @@
       <c r="H3">
         <v>0.98053100000000004</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="13">
         <f t="shared" ref="I3:I10" si="0">AVERAGE(D3:H3)</f>
         <v>0.96077139999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>0.39718500000000001</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>0.39888600000000002</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>0.40608299999999897</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>0.38511499999999999</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="6">
         <v>0.39600400000000002</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="13">
         <f t="shared" si="0"/>
         <v>0.39665459999999975</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5">
@@ -5011,14 +5000,14 @@
       <c r="H5">
         <v>1.1860000000000199E-3</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="13">
         <f t="shared" si="0"/>
         <v>1.1647999999999982E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
+    <row r="6" spans="1:9">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D6">
@@ -5030,129 +5019,129 @@
       <c r="F6">
         <v>3.5150000000000398E-3</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="8">
         <v>3.5659999999999499E-3</v>
       </c>
       <c r="H6">
         <v>3.40099999999998E-3</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="13">
         <f t="shared" si="0"/>
         <v>3.4699999999999653E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>1.4240000000000301E-3</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <v>1.48400000000004E-3</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <v>1.4089999999999899E-3</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <v>1.45699999999998E-3</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="6">
         <v>1.59899999999996E-3</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="13">
         <f t="shared" si="0"/>
         <v>1.4746E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:9">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>1.6410999999999999E-2</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>1.63329999999999E-2</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <v>1.6601999999999999E-2</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="8">
         <v>1.6722000000000001E-2</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="8">
         <v>1.6666E-2</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="11">
         <f t="shared" si="0"/>
         <v>1.654679999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" s="8"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <v>5.0868999999999998E-2</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <v>5.0996999999999897E-2</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="8">
         <v>5.0644000000000002E-2</v>
       </c>
       <c r="G9">
         <v>5.2000999999999901E-2</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="8">
         <v>5.1580000000000001E-2</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="11">
         <f t="shared" si="0"/>
         <v>5.1218199999999957E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="12" t="s">
+    <row r="10" spans="1:9">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="14">
         <v>2.0684999999999999E-2</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="14">
         <v>2.0639000000000001E-2</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="14">
         <v>2.2311999999999999E-2</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="14">
         <v>2.0962999999999999E-2</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="14">
         <v>2.0702999999999899E-2</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="15">
         <f t="shared" si="0"/>
         <v>2.1060399999999979E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="B15" t="str">
         <f>B2</f>
-        <v>Shakespear</v>
+        <v>Shakespeare</v>
       </c>
       <c r="C15" t="str">
         <f>B8</f>
@@ -5163,7 +5152,7 @@
         <v>Lottery</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" t="str" cm="1">
         <f t="array" ref="A16:A18">C2:C4</f>
         <v>Boyer Moore</v>
@@ -5181,7 +5170,7 @@
         <v>1.1647999999999982E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="str">
         <v>Rabin Karp</v>
       </c>
@@ -5195,7 +5184,7 @@
         <v>3.4699999999999653E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="str">
         <v>Brute Force</v>
       </c>

</xml_diff>

<commit_message>
axis label for graphs
</commit_message>
<xml_diff>
--- a/CSC430 Proj.xlsx
+++ b/CSC430 Proj.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/logancamp/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/logancamp/Desktop/CSC430/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F9672A-A651-2449-B84E-1FF31CE8DEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A739F88A-D428-7D4B-84C2-73CF124F0EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{194B7978-61BF-E746-BFF1-312F519DEFB4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22340" xr2:uid="{194B7978-61BF-E746-BFF1-312F519DEFB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -250,11 +250,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -265,9 +262,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -275,12 +269,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,6 +665,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1642,6 +1693,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2124,6 +2230,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4875,8 +5036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3516C63E-AE4E-114B-B95F-EE1600AC9405}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4888,20 +5049,20 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="14" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4909,10 +5070,10 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2">
@@ -4930,14 +5091,14 @@
       <c r="H2">
         <v>0.30901499999999998</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="12">
         <f>AVERAGE(D2:H2)</f>
         <v>0.30481060000000004</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D3">
@@ -4955,33 +5116,33 @@
       <c r="H3">
         <v>0.98053100000000004</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="12">
         <f t="shared" ref="I3:I10" si="0">AVERAGE(D3:H3)</f>
         <v>0.96077139999999994</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>0.39718500000000001</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>0.39888600000000002</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>0.40608299999999897</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>0.38511499999999999</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="6">
         <v>0.39600400000000002</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="12">
         <f t="shared" si="0"/>
         <v>0.39665459999999975</v>
       </c>
@@ -4990,10 +5151,10 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5">
@@ -5011,14 +5172,14 @@
       <c r="H5">
         <v>1.1860000000000199E-3</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="12">
         <f t="shared" si="0"/>
         <v>1.1647999999999982E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D6">
@@ -5030,121 +5191,121 @@
       <c r="F6">
         <v>3.5150000000000398E-3</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="8">
         <v>3.5659999999999499E-3</v>
       </c>
       <c r="H6">
         <v>3.40099999999998E-3</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="12">
         <f t="shared" si="0"/>
         <v>3.4699999999999653E-3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>1.4240000000000301E-3</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <v>1.48400000000004E-3</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <v>1.4089999999999899E-3</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <v>1.45699999999998E-3</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="6">
         <v>1.59899999999996E-3</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="12">
         <f t="shared" si="0"/>
         <v>1.4746E-3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>1.6410999999999999E-2</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>1.63329999999999E-2</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <v>1.6601999999999999E-2</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="8">
         <v>1.6722000000000001E-2</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="8">
         <v>1.6666E-2</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="11">
         <f t="shared" si="0"/>
         <v>1.654679999999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <v>5.0868999999999998E-2</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <v>5.0996999999999897E-2</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="8">
         <v>5.0644000000000002E-2</v>
       </c>
       <c r="G9">
         <v>5.2000999999999901E-2</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="8">
         <v>5.1580000000000001E-2</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="11">
         <f t="shared" si="0"/>
         <v>5.1218199999999957E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="12" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="8">
         <v>2.0684999999999999E-2</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="8">
         <v>2.0639000000000001E-2</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="8">
         <v>2.2311999999999999E-2</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="8">
         <v>2.0962999999999999E-2</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="8">
         <v>2.0702999999999899E-2</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="13">
         <f t="shared" si="0"/>
         <v>2.1060399999999979E-2</v>
       </c>

</xml_diff>

<commit_message>
added seconds label again
</commit_message>
<xml_diff>
--- a/CSC430 Proj.xlsx
+++ b/CSC430 Proj.xlsx
@@ -1,38 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonyj\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/logancamp/Desktop/CSC430/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352F258F-7AB4-47B4-B247-D7A1C2EFCF7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EF4E08-2AAD-B648-86FF-BD74A65F55A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{194B7978-61BF-E746-BFF1-312F519DEFB4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33720" windowHeight="18040" xr2:uid="{194B7978-61BF-E746-BFF1-312F519DEFB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -89,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -239,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,9 +259,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -262,7 +270,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -658,6 +665,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1147,6 +1209,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1631,6 +1748,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2113,6 +2285,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4864,41 +5091,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3516C63E-AE4E-114B-B95F-EE1600AC9405}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="99" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="12" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -4919,12 +5146,12 @@
       <c r="H2">
         <v>0.30901499999999998</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="12">
         <f>AVERAGE(D2:H2)</f>
         <v>0.30481060000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -4944,38 +5171,38 @@
       <c r="H3">
         <v>0.98053100000000004</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <f t="shared" ref="I3:I10" si="0">AVERAGE(D3:H3)</f>
         <v>0.96077139999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>0.39718500000000001</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>0.39888600000000002</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>0.40608299999999897</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>0.38511499999999999</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>0.39600400000000002</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <f t="shared" si="0"/>
         <v>0.39665459999999975</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -5000,12 +5227,12 @@
       <c r="H5">
         <v>1.1860000000000199E-3</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <f t="shared" si="0"/>
         <v>1.1647999999999982E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
         <v>2</v>
@@ -5019,126 +5246,126 @@
       <c r="F6">
         <v>3.5150000000000398E-3</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>3.5659999999999499E-3</v>
       </c>
       <c r="H6">
         <v>3.40099999999998E-3</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="12">
         <f t="shared" si="0"/>
         <v>3.4699999999999653E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>1.4240000000000301E-3</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>1.48400000000004E-3</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>1.4089999999999899E-3</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>1.45699999999998E-3</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>1.59899999999996E-3</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <f t="shared" si="0"/>
         <v>1.4746E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>1.6410999999999999E-2</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>1.63329999999999E-2</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>1.6601999999999999E-2</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>1.6722000000000001E-2</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>1.6666E-2</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <f t="shared" si="0"/>
         <v>1.654679999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="8"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="9" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>5.0868999999999998E-2</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>5.0996999999999897E-2</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>5.0644000000000002E-2</v>
       </c>
       <c r="G9">
         <v>5.2000999999999901E-2</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>5.1580000000000001E-2</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <f t="shared" si="0"/>
         <v>5.1218199999999957E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="10" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="7">
         <v>2.0684999999999999E-2</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="7">
         <v>2.0639000000000001E-2</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="7">
         <v>2.2311999999999999E-2</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="7">
         <v>2.0962999999999999E-2</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="7">
         <v>2.0702999999999899E-2</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="13">
         <f t="shared" si="0"/>
         <v>2.1060399999999979E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="str">
         <f>B2</f>
         <v>Shakespeare</v>
@@ -5152,7 +5379,7 @@
         <v>Lottery</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="str" cm="1">
         <f t="array" ref="A16:A18">C2:C4</f>
         <v>Boyer Moore</v>
@@ -5170,7 +5397,7 @@
         <v>1.1647999999999982E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <v>Rabin Karp</v>
       </c>
@@ -5184,7 +5411,7 @@
         <v>3.4699999999999653E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <v>Brute Force</v>
       </c>

</xml_diff>